<commit_message>
Some testing was done Implementing also a function called is_diagonally_dominant for checking is the matrix is valid to apply the method
</commit_message>
<xml_diff>
--- a/data/File.xlsx
+++ b/data/File.xlsx
@@ -34,13 +34,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -72,22 +72,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -391,7 +388,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -401,10 +398,10 @@
     <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,49 +411,72 @@
       <c r="E1" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="3">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="A2" s="1">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
         <v>24</v>
       </c>
-      <c r="E2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="3">
+        <v>-1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3">
-        <v>3</v>
-      </c>
-      <c r="D3" s="3">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="3">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes to the matrix
</commit_message>
<xml_diff>
--- a/data/File.xlsx
+++ b/data/File.xlsx
@@ -72,19 +72,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -388,17 +397,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -409,73 +420,145 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="B2" s="1">
-        <v>4</v>
+        <v>-22</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>-66</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="3">
-        <v>24</v>
+      <c r="E2" s="4">
+        <v>2</v>
+      </c>
+      <c r="F2" s="4">
+        <v>-4</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>5</v>
+        <v>-26</v>
       </c>
       <c r="C3" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
+        <v>-7</v>
+      </c>
+      <c r="F3" s="4">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>-8</v>
+      </c>
+      <c r="G4" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3">
-        <v>-1</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3">
-        <v>6</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="1">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>4</v>
-      </c>
-      <c r="E5" s="3">
-        <v>2</v>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
+        <v>45</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="5">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>